<commit_message>
sales add jQuery done ....
</commit_message>
<xml_diff>
--- a/SISTEM-TOKO-MAJU-ONLINE.xlsx
+++ b/SISTEM-TOKO-MAJU-ONLINE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="102">
   <si>
     <t>SUSUNAN MASTER DAN TABEL SISTEM TOKO MAJU</t>
   </si>
@@ -198,12 +198,6 @@
     <t>Hutang / Rekening Koran (terhadap supplier) (utk setiap PO)</t>
   </si>
   <si>
-    <t>Credit (Beban Hutang)</t>
-  </si>
-  <si>
-    <t>Debit (Bayar Hutang)</t>
-  </si>
-  <si>
     <t>Nomer / kode referensi bukti pembayaran</t>
   </si>
   <si>
@@ -324,14 +318,17 @@
     <t>Sales Order (SO)</t>
   </si>
   <si>
-    <t>History pembelian (menampilkan seluruh SO oleh customer tsb)</t>
+    <t>Debit / Mutasi Debet (Bayar Hutang)</t>
+  </si>
+  <si>
+    <t>Credit / Mutasi Kredit (Beban Hutang)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -640,156 +637,162 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,7 +882,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -914,7 +916,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1090,14 +1091,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55:G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="3" width="20.28515625" customWidth="1"/>
@@ -1107,26 +1108,26 @@
     <col min="10" max="10" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:8" ht="23.25">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
       <c r="H1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75">
       <c r="A2" s="25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1149,8 +1150,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="48" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1172,8 +1173,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63"/>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="49"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1186,15 +1187,15 @@
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="51" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="63"/>
+    <row r="6" spans="1:8">
+      <c r="A6" s="49"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1207,13 +1208,13 @@
       <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="75" t="s">
+      <c r="F6" s="51"/>
+      <c r="G6" s="45" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
+    <row r="7" spans="1:8">
+      <c r="A7" s="49"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1226,11 +1227,11 @@
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="75"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="63"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="45"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="49"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1243,13 +1244,13 @@
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="51"/>
       <c r="G8" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
+    <row r="9" spans="1:8">
+      <c r="A9" s="49"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1262,13 +1263,13 @@
       <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="51"/>
       <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="63"/>
+    <row r="10" spans="1:8">
+      <c r="A10" s="49"/>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1281,13 +1282,13 @@
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="51"/>
       <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="63"/>
+    <row r="11" spans="1:8" ht="15" customHeight="1">
+      <c r="A11" s="49"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1300,14 +1301,14 @@
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="51"/>
       <c r="G11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A12" s="49"/>
+      <c r="B12" s="90" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1316,207 +1317,205 @@
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="75" t="s">
+      <c r="E12" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="51"/>
+      <c r="G12" s="45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
-      <c r="B13" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="41" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="49"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="76"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="75"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="63"/>
-      <c r="B14" s="76"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="76" t="s">
+      <c r="E13" s="46"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="45"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="49"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="46" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="76"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="76"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="63"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="76"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="63"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="76"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="77"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
+      <c r="A15" s="49"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="46"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="49"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="46"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="49"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="46"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A18" s="50"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="47"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.75">
       <c r="A20" s="25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="31.5" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="52" t="s">
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="53"/>
-      <c r="G21" s="50" t="s">
+      <c r="F21" s="80"/>
+      <c r="G21" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="51"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="s">
+      <c r="H21" s="78"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="88" t="s">
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="89"/>
-      <c r="G22" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="40"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63"/>
-      <c r="B23" s="32" t="s">
+      <c r="F22" s="44"/>
+      <c r="G22" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="55"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="A23" s="49"/>
+      <c r="B23" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="26" t="s">
+      <c r="C23" s="57"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="81" t="s">
+      <c r="F23" s="35"/>
+      <c r="G23" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="82"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="63"/>
-      <c r="B24" s="32" t="s">
+      <c r="H23" s="33"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1">
+      <c r="A24" s="49"/>
+      <c r="B24" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="26" t="s">
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="86" t="s">
+      <c r="F24" s="35"/>
+      <c r="G24" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="H24" s="87"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="63"/>
-      <c r="B25" s="69" t="s">
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="49"/>
+      <c r="B25" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="70"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="26" t="s">
+      <c r="C25" s="60"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="87"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="63"/>
-      <c r="B26" s="58" t="s">
+      <c r="F25" s="35"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="42"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1">
+      <c r="A26" s="49"/>
+      <c r="B26" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="26" t="s">
+      <c r="C26" s="74"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="28"/>
-      <c r="G26" s="86"/>
-      <c r="H26" s="87"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="63"/>
-      <c r="B27" s="32" t="s">
+      <c r="F26" s="35"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="42"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="49"/>
+      <c r="B27" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" s="44"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="63"/>
-      <c r="B28" s="83" t="s">
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="40"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="49"/>
+      <c r="B28" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="84"/>
-      <c r="D28" s="85"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="H28" s="44"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="63"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28" s="40"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1">
+      <c r="A29" s="49"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
@@ -1526,15 +1525,15 @@
       <c r="D29" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="86" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="87"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="63"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="42"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="49"/>
       <c r="B30" s="3" t="s">
         <v>48</v>
       </c>
@@ -1544,13 +1543,13 @@
       <c r="D30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="26"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="86"/>
-      <c r="H30" s="87"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="63"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="42"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="49"/>
       <c r="B31" s="11" t="s">
         <v>45</v>
       </c>
@@ -1560,13 +1559,13 @@
       <c r="D31" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="42"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="87"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="63"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="42"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="49"/>
       <c r="B32" s="11" t="s">
         <v>49</v>
       </c>
@@ -1576,13 +1575,13 @@
       <c r="D32" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="44"/>
-    </row>
-    <row r="33" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="63"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="40"/>
+    </row>
+    <row r="33" spans="1:10" ht="32.25" customHeight="1">
+      <c r="A33" s="49"/>
       <c r="B33" s="12" t="s">
         <v>50</v>
       </c>
@@ -1592,13 +1591,13 @@
       <c r="D33" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="42"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="44"/>
-    </row>
-    <row r="34" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="63"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="40"/>
+    </row>
+    <row r="34" spans="1:10" ht="31.5" customHeight="1">
+      <c r="A34" s="49"/>
       <c r="B34" s="13" t="s">
         <v>51</v>
       </c>
@@ -1608,189 +1607,189 @@
       <c r="D34" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="42"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="44"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="63"/>
-      <c r="B35" s="78" t="s">
+      <c r="E34" s="39"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="40"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="49"/>
+      <c r="B35" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="44"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="65"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="48"/>
-    </row>
-    <row r="38" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C35" s="30"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="40"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="50"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="64"/>
+    </row>
+    <row r="38" spans="1:10" ht="18.75">
       <c r="A38" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30.75" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="52" t="s">
-        <v>65</v>
-      </c>
-      <c r="F39" s="57"/>
-      <c r="G39" s="53"/>
+      <c r="B39" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="84"/>
+      <c r="G39" s="80"/>
       <c r="H39" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="40"/>
-      <c r="E40" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="54"/>
+      <c r="G40" s="55"/>
       <c r="H40" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="63"/>
-      <c r="B41" s="32" t="s">
+    <row r="41" spans="1:10">
+      <c r="A41" s="49"/>
+      <c r="B41" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="33"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="F41" s="33"/>
-      <c r="G41" s="34"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="F41" s="57"/>
+      <c r="G41" s="58"/>
       <c r="H41" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>57</v>
       </c>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="63"/>
-      <c r="B42" s="32" t="s">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A42" s="49"/>
+      <c r="B42" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="F42" s="67"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="I42" s="41" t="s">
+      <c r="C42" s="57"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="68"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="I42" s="51" t="s">
         <v>58</v>
       </c>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="63"/>
-      <c r="B43" s="69" t="s">
+    <row r="43" spans="1:10">
+      <c r="A43" s="49"/>
+      <c r="B43" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="70"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="32" t="s">
+      <c r="C43" s="60"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="33"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="63"/>
-      <c r="B44" s="58" t="s">
+    <row r="44" spans="1:10">
+      <c r="A44" s="49"/>
+      <c r="B44" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="F44" s="73"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
+      <c r="C44" s="74"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="71"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="63"/>
-      <c r="B45" s="32" t="s">
+    <row r="45" spans="1:10">
+      <c r="A45" s="49"/>
+      <c r="B45" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="33"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="I45" s="41"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="I45" s="51"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="63"/>
-      <c r="B46" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="F46" s="55"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="41"/>
+    <row r="46" spans="1:10">
+      <c r="A46" s="49"/>
+      <c r="B46" s="81" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="82"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="81" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="82"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="51"/>
       <c r="I46" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="63"/>
+    <row r="47" spans="1:10" ht="15" customHeight="1">
+      <c r="A47" s="49"/>
       <c r="B47" s="10" t="s">
         <v>44</v>
       </c>
@@ -1809,14 +1808,14 @@
       <c r="G47" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H47" s="41"/>
+      <c r="H47" s="51"/>
       <c r="I47" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="63"/>
+    <row r="48" spans="1:10" ht="15" customHeight="1">
+      <c r="A48" s="49"/>
       <c r="B48" s="3" t="s">
         <v>48</v>
       </c>
@@ -1835,16 +1834,16 @@
       <c r="G48" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H48" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="I48" s="41" t="s">
-        <v>63</v>
+      <c r="H48" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="I48" s="51" t="s">
+        <v>61</v>
       </c>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="63"/>
+    <row r="49" spans="1:10">
+      <c r="A49" s="49"/>
       <c r="B49" s="11" t="s">
         <v>45</v>
       </c>
@@ -1855,20 +1854,20 @@
         <v>45</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
+        <v>78</v>
+      </c>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
       <c r="J49" s="7"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="63"/>
+    <row r="50" spans="1:10">
+      <c r="A50" s="49"/>
       <c r="B50" s="11" t="s">
         <v>30</v>
       </c>
@@ -1878,54 +1877,54 @@
       <c r="D50" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E50" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="F50" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="G50" s="41" t="s">
-        <v>81</v>
+      <c r="E50" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="G50" s="51" t="s">
+        <v>79</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="63"/>
+    <row r="51" spans="1:10">
+      <c r="A51" s="49"/>
       <c r="B51" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
+        <v>66</v>
+      </c>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
       <c r="H51" s="5"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="63"/>
+    <row r="52" spans="1:10">
+      <c r="A52" s="49"/>
       <c r="B52" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" s="45"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="45"/>
+        <v>67</v>
+      </c>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
+      <c r="G52" s="52"/>
       <c r="H52" s="5"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="63"/>
+    <row r="53" spans="1:10" ht="30">
+      <c r="A53" s="49"/>
       <c r="B53" s="12" t="s">
         <v>50</v>
       </c>
@@ -1935,14 +1934,14 @@
       <c r="D53" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E53" s="26"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="28"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="35"/>
       <c r="H53" s="5"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="63"/>
+    <row r="54" spans="1:10" ht="30">
+      <c r="A54" s="49"/>
       <c r="B54" s="12" t="s">
         <v>51</v>
       </c>
@@ -1952,226 +1951,247 @@
       <c r="D54" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E54" s="42"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="44"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="65"/>
+      <c r="G54" s="40"/>
       <c r="H54" s="5"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="63"/>
-      <c r="B55" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="39"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="44"/>
+    <row r="55" spans="1:10">
+      <c r="A55" s="49"/>
+      <c r="B55" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="54"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="40"/>
       <c r="H55" s="5"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="63"/>
-      <c r="B56" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" s="46"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="44"/>
+    <row r="56" spans="1:10">
+      <c r="A56" s="49"/>
+      <c r="B56" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="86"/>
+      <c r="D56" s="58"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="65"/>
+      <c r="G56" s="40"/>
       <c r="H56" s="5"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="64"/>
-      <c r="B57" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="33"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="44"/>
+    <row r="57" spans="1:10">
+      <c r="A57" s="66"/>
+      <c r="B57" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="57"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="65"/>
+      <c r="G57" s="40"/>
       <c r="H57" s="5"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="63"/>
-      <c r="B58" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="44"/>
+    <row r="58" spans="1:10">
+      <c r="A58" s="49"/>
+      <c r="B58" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="65"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="65"/>
+      <c r="G58" s="40"/>
       <c r="H58" s="5"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="63"/>
-      <c r="B59" s="42" t="s">
+    <row r="59" spans="1:10">
+      <c r="A59" s="49"/>
+      <c r="B59" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C59" s="43"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="44"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="40"/>
       <c r="H59" s="5"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="63"/>
-      <c r="B60" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="C60" s="43"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="44"/>
+    <row r="60" spans="1:10">
+      <c r="A60" s="49"/>
+      <c r="B60" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" s="65"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="65"/>
+      <c r="G60" s="40"/>
       <c r="H60" s="5"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="65"/>
-      <c r="B61" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="C61" s="61"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="48"/>
+    <row r="61" spans="1:10">
+      <c r="A61" s="50"/>
+      <c r="B61" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="63"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="64"/>
       <c r="H61" s="6"/>
       <c r="I61" s="14"/>
     </row>
-    <row r="63" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="18.75">
       <c r="A63" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B64" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="37"/>
+      <c r="B64" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="27"/>
+      <c r="D64" s="28"/>
       <c r="G64" s="16"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="B65" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="39"/>
-      <c r="D65" s="40"/>
+      <c r="C65" s="54"/>
+      <c r="D65" s="55"/>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66" s="21"/>
       <c r="B66" s="22"/>
       <c r="C66" s="23"/>
       <c r="D66" s="24"/>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="85"/>
+      <c r="D67" s="35"/>
+      <c r="G67" s="9"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="1"/>
+      <c r="B68" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68" s="85"/>
+      <c r="D68" s="35"/>
+      <c r="G68" s="9"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="1"/>
+      <c r="B69" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69" s="57"/>
+      <c r="D69" s="58"/>
+      <c r="G69" s="9"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="1"/>
+      <c r="B70" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="B67" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C67" s="27"/>
-      <c r="D67" s="28"/>
-      <c r="G67" s="9"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C68" s="27"/>
-      <c r="D68" s="28"/>
-      <c r="G68" s="9"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="32" t="s">
+      <c r="C70" s="85"/>
+      <c r="D70" s="35"/>
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="1"/>
+      <c r="B71" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" s="85"/>
+      <c r="D71" s="35"/>
+      <c r="G71" s="16"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="14"/>
+      <c r="B72" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="C69" s="33"/>
-      <c r="D69" s="34"/>
-      <c r="G69" s="9"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C70" s="27"/>
-      <c r="D70" s="28"/>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C71" s="27"/>
-      <c r="D71" s="28"/>
-      <c r="G71" s="16"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" s="30"/>
-      <c r="D72" s="31"/>
+      <c r="C72" s="88"/>
+      <c r="D72" s="89"/>
       <c r="G72" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G24:H26"/>
-    <mergeCell ref="G29:H31"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="A22:A36"/>
-    <mergeCell ref="A4:A18"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="D13:D18"/>
-    <mergeCell ref="E12:E18"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F5:F18"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="I42:I45"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="H45:H47"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E60:G60"/>
     <mergeCell ref="E55:G55"/>
     <mergeCell ref="E56:G56"/>
     <mergeCell ref="E57:G57"/>
@@ -2188,57 +2208,36 @@
     <mergeCell ref="E45:G45"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="I42:I45"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="H45:H47"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="A22:A36"/>
+    <mergeCell ref="A4:A18"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="D13:D18"/>
+    <mergeCell ref="E12:E18"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F5:F18"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G24:H26"/>
+    <mergeCell ref="G29:H31"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E35:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2246,24 +2245,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>